<commit_message>
add Hospital for Tropical Diseases
</commit_message>
<xml_diff>
--- a/labs.xlsx
+++ b/labs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="501">
   <si>
     <t>LAB</t>
   </si>
@@ -1508,6 +1508,15 @@
   </si>
   <si>
     <t>Sarah Gabriel</t>
+  </si>
+  <si>
+    <t>+44 20 3447 5418</t>
+  </si>
+  <si>
+    <t>Prof PL Chiodini</t>
+  </si>
+  <si>
+    <t>p.chiodini@nhs.net</t>
   </si>
 </sst>
 </file>
@@ -1578,19 +1587,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="24">
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1791,6 +1787,19 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -1814,14 +1823,14 @@
     <tableColumn id="1" name="LAB"/>
     <tableColumn id="15" name="URL"/>
     <tableColumn id="2" name="STREET"/>
-    <tableColumn id="7" name="ZIP" dataDxfId="3"/>
+    <tableColumn id="7" name="ZIP" dataDxfId="23"/>
     <tableColumn id="14" name="CITY"/>
     <tableColumn id="17" name="COUNTRY"/>
-    <tableColumn id="3" name="TEL" dataDxfId="2"/>
+    <tableColumn id="3" name="TEL" dataDxfId="22"/>
     <tableColumn id="4" name="CONTACT"/>
     <tableColumn id="5" name="EMAIL" dataCellStyle="Hyperlink"/>
-    <tableColumn id="16" name="LAT" dataDxfId="1"/>
-    <tableColumn id="6" name="LONG" dataDxfId="0"/>
+    <tableColumn id="16" name="LAT" dataDxfId="21"/>
+    <tableColumn id="6" name="LONG" dataDxfId="20"/>
     <tableColumn id="12" name="TSOL_CC_AB"/>
     <tableColumn id="13" name="TSOL_CC_AG"/>
     <tableColumn id="8" name="TSOL_HT"/>
@@ -2122,8 +2131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5744,9 +5753,21 @@
       <c r="F75" t="s">
         <v>102</v>
       </c>
-      <c r="I75" s="1"/>
-      <c r="J75" s="2"/>
-      <c r="K75" s="2"/>
+      <c r="G75" s="4" t="s">
+        <v>498</v>
+      </c>
+      <c r="H75" t="s">
+        <v>499</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="J75" s="2">
+        <v>51.522748</v>
+      </c>
+      <c r="K75" s="2">
+        <v>-0.13553780000000001</v>
+      </c>
       <c r="L75" t="s">
         <v>9</v>
       </c>
@@ -5821,82 +5842,82 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L2:P17 L18:O54">
-    <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P18:P54">
-    <cfRule type="cellIs" dxfId="21" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P55:P73">
-    <cfRule type="cellIs" dxfId="19" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L55:O73">
-    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P74">
-    <cfRule type="cellIs" dxfId="15" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L74:O74">
-    <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L75:O75">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P75">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L76:O76">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P76">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5924,11 +5945,12 @@
     <hyperlink ref="B75" r:id="rId16"/>
     <hyperlink ref="B76" r:id="rId17"/>
     <hyperlink ref="I76" r:id="rId18"/>
+    <hyperlink ref="I75" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
   <tableParts count="1">
-    <tablePart r:id="rId20"/>
+    <tablePart r:id="rId21"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>